<commit_message>
Update phân công viết SRS
</commit_message>
<xml_diff>
--- a/TÀI LIỆU/Phân chia công việc và tiến độ dự án.xlsx
+++ b/TÀI LIỆU/Phân chia công việc và tiến độ dự án.xlsx
@@ -1,21 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22527"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Administrator\Desktop\DoAnChuyenNganh\MangXaHoiViecLamIT\TÀI LIỆU\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin\Desktop\MangXaHoiViecLamIT\TÀI LIỆU\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A4A11AA-18A6-40DC-93F5-A5F05685B1E9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456"/>
   </bookViews>
   <sheets>
     <sheet name="GanttChart" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -28,12 +27,12 @@
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
     <author/>
   </authors>
   <commentList>
-    <comment ref="A7" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000001000000}">
+    <comment ref="A7" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -50,7 +49,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B7" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000002000000}">
+    <comment ref="B7" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -64,7 +63,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C7" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000003000000}">
+    <comment ref="C7" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -78,7 +77,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D7" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000004000000}">
+    <comment ref="D7" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -92,7 +91,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E7" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000005000000}">
+    <comment ref="E7" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -106,7 +105,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F7" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000006000000}">
+    <comment ref="F7" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -120,7 +119,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="G7" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000007000000}">
+    <comment ref="G7" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -134,7 +133,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="H7" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000008000000}">
+    <comment ref="H7" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -153,7 +152,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="61">
   <si>
     <t>Ngày bắt đầu dự án:</t>
   </si>
@@ -320,12 +319,33 @@
   </si>
   <si>
     <t>Review code</t>
+  </si>
+  <si>
+    <t>Phân tích các chức năng cho nhà tuyển dụng: Đăng ký, đăng nhập, tạo hoặc chỉnh sửa hồ sơ, đăng bài tuyển dụng</t>
+  </si>
+  <si>
+    <t>Phân tích các chức năng cho ứng viên: Đăng ký, Đăng nhập, đăng CV, tìm việc bằng chữ với ô tìm kiếm</t>
+  </si>
+  <si>
+    <t>Phân tích chức năng cho ứng viên: Tìm việc bằng chức năng lọc, ứng tuyển công việc, viết review về công ty</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Phân tích và vẽ usecase diagram </t>
+  </si>
+  <si>
+    <t>Ngyễn An Toàn</t>
+  </si>
+  <si>
+    <t>04/21/2022</t>
+  </si>
+  <si>
+    <t>04/23/2022</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="4">
     <numFmt numFmtId="164" formatCode="m/d/yyyy\ \(dddd\)"/>
     <numFmt numFmtId="165" formatCode="d\ mmm\ yyyy"/>
@@ -644,6 +664,28 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -652,28 +694,6 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -931,22 +951,22 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
   <dimension ref="A1:BM43"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane ySplit="7" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G44" sqref="G44"/>
+      <pane ySplit="7" topLeftCell="A9" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="11.6640625" style="21" customWidth="1"/>
-    <col min="2" max="2" width="35.21875" style="21" customWidth="1"/>
-    <col min="3" max="3" width="29.6640625" style="21" customWidth="1"/>
+    <col min="2" max="2" width="120.77734375" style="21" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="26.44140625" style="21" customWidth="1"/>
     <col min="4" max="5" width="13.77734375" style="21" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="9.5546875" style="21" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="15.5546875" style="21" bestFit="1" customWidth="1"/>
@@ -966,68 +986,68 @@
       </c>
       <c r="B1" s="20"/>
       <c r="C1" s="20"/>
-      <c r="D1" s="48"/>
-      <c r="E1" s="48"/>
-      <c r="F1" s="48"/>
-      <c r="G1" s="48"/>
-      <c r="H1" s="48"/>
-      <c r="I1" s="48"/>
-      <c r="J1" s="48"/>
-      <c r="K1" s="48"/>
-      <c r="L1" s="48"/>
-      <c r="M1" s="48"/>
-      <c r="N1" s="48"/>
-      <c r="O1" s="48"/>
-      <c r="P1" s="48"/>
-      <c r="Q1" s="48"/>
-      <c r="R1" s="48"/>
-      <c r="S1" s="48"/>
-      <c r="T1" s="48"/>
-      <c r="U1" s="48"/>
-      <c r="V1" s="48"/>
-      <c r="W1" s="48"/>
-      <c r="X1" s="48"/>
-      <c r="Y1" s="48"/>
-      <c r="Z1" s="48"/>
-      <c r="AA1" s="48"/>
-      <c r="AB1" s="48"/>
-      <c r="AC1" s="48"/>
-      <c r="AD1" s="48"/>
-      <c r="AE1" s="48"/>
-      <c r="AF1" s="48"/>
-      <c r="AG1" s="48"/>
-      <c r="AH1" s="48"/>
-      <c r="AI1" s="48"/>
-      <c r="AJ1" s="48"/>
-      <c r="AK1" s="48"/>
-      <c r="AL1" s="48"/>
-      <c r="AM1" s="48"/>
-      <c r="AN1" s="48"/>
-      <c r="AO1" s="48"/>
-      <c r="AP1" s="48"/>
-      <c r="AQ1" s="48"/>
-      <c r="AR1" s="48"/>
-      <c r="AS1" s="48"/>
-      <c r="AT1" s="48"/>
-      <c r="AU1" s="48"/>
-      <c r="AV1" s="48"/>
-      <c r="AW1" s="48"/>
-      <c r="AX1" s="48"/>
-      <c r="AY1" s="48"/>
-      <c r="AZ1" s="48"/>
-      <c r="BA1" s="48"/>
-      <c r="BB1" s="48"/>
-      <c r="BC1" s="48"/>
-      <c r="BD1" s="48"/>
-      <c r="BE1" s="48"/>
-      <c r="BF1" s="48"/>
-      <c r="BG1" s="48"/>
-      <c r="BH1" s="48"/>
-      <c r="BI1" s="48"/>
-      <c r="BJ1" s="48"/>
-      <c r="BK1" s="48"/>
-      <c r="BL1" s="48"/>
-      <c r="BM1" s="48"/>
+      <c r="D1" s="37"/>
+      <c r="E1" s="37"/>
+      <c r="F1" s="37"/>
+      <c r="G1" s="37"/>
+      <c r="H1" s="37"/>
+      <c r="I1" s="37"/>
+      <c r="J1" s="37"/>
+      <c r="K1" s="37"/>
+      <c r="L1" s="37"/>
+      <c r="M1" s="37"/>
+      <c r="N1" s="37"/>
+      <c r="O1" s="37"/>
+      <c r="P1" s="37"/>
+      <c r="Q1" s="37"/>
+      <c r="R1" s="37"/>
+      <c r="S1" s="37"/>
+      <c r="T1" s="37"/>
+      <c r="U1" s="37"/>
+      <c r="V1" s="37"/>
+      <c r="W1" s="37"/>
+      <c r="X1" s="37"/>
+      <c r="Y1" s="37"/>
+      <c r="Z1" s="37"/>
+      <c r="AA1" s="37"/>
+      <c r="AB1" s="37"/>
+      <c r="AC1" s="37"/>
+      <c r="AD1" s="37"/>
+      <c r="AE1" s="37"/>
+      <c r="AF1" s="37"/>
+      <c r="AG1" s="37"/>
+      <c r="AH1" s="37"/>
+      <c r="AI1" s="37"/>
+      <c r="AJ1" s="37"/>
+      <c r="AK1" s="37"/>
+      <c r="AL1" s="37"/>
+      <c r="AM1" s="37"/>
+      <c r="AN1" s="37"/>
+      <c r="AO1" s="37"/>
+      <c r="AP1" s="37"/>
+      <c r="AQ1" s="37"/>
+      <c r="AR1" s="37"/>
+      <c r="AS1" s="37"/>
+      <c r="AT1" s="37"/>
+      <c r="AU1" s="37"/>
+      <c r="AV1" s="37"/>
+      <c r="AW1" s="37"/>
+      <c r="AX1" s="37"/>
+      <c r="AY1" s="37"/>
+      <c r="AZ1" s="37"/>
+      <c r="BA1" s="37"/>
+      <c r="BB1" s="37"/>
+      <c r="BC1" s="37"/>
+      <c r="BD1" s="37"/>
+      <c r="BE1" s="37"/>
+      <c r="BF1" s="37"/>
+      <c r="BG1" s="37"/>
+      <c r="BH1" s="37"/>
+      <c r="BI1" s="37"/>
+      <c r="BJ1" s="37"/>
+      <c r="BK1" s="37"/>
+      <c r="BL1" s="37"/>
+      <c r="BM1" s="37"/>
     </row>
     <row r="2" spans="1:65" ht="15" x14ac:dyDescent="0.25">
       <c r="A2" s="22" t="s">
@@ -1167,15 +1187,15 @@
     </row>
     <row r="4" spans="1:65" ht="15" x14ac:dyDescent="0.25">
       <c r="A4" s="24"/>
-      <c r="B4" s="43" t="s">
+      <c r="B4" s="40" t="s">
         <v>0</v>
       </c>
       <c r="C4" s="41"/>
-      <c r="D4" s="49">
+      <c r="D4" s="38">
         <v>44641</v>
       </c>
-      <c r="E4" s="46"/>
-      <c r="F4" s="43" t="s">
+      <c r="E4" s="39"/>
+      <c r="F4" s="40" t="s">
         <v>1</v>
       </c>
       <c r="G4" s="41"/>
@@ -1183,7 +1203,7 @@
         <v>1</v>
       </c>
       <c r="I4" s="24"/>
-      <c r="J4" s="47" t="s">
+      <c r="J4" s="42" t="s">
         <v>2</v>
       </c>
       <c r="K4" s="41"/>
@@ -1191,8 +1211,8 @@
       <c r="M4" s="41"/>
       <c r="N4" s="41"/>
       <c r="O4" s="41"/>
-      <c r="P4" s="42"/>
-      <c r="Q4" s="47" t="s">
+      <c r="P4" s="43"/>
+      <c r="Q4" s="42" t="s">
         <v>3</v>
       </c>
       <c r="R4" s="41"/>
@@ -1200,8 +1220,8 @@
       <c r="T4" s="41"/>
       <c r="U4" s="41"/>
       <c r="V4" s="41"/>
-      <c r="W4" s="42"/>
-      <c r="X4" s="47" t="s">
+      <c r="W4" s="43"/>
+      <c r="X4" s="42" t="s">
         <v>4</v>
       </c>
       <c r="Y4" s="41"/>
@@ -1209,8 +1229,8 @@
       <c r="AA4" s="41"/>
       <c r="AB4" s="41"/>
       <c r="AC4" s="41"/>
-      <c r="AD4" s="42"/>
-      <c r="AE4" s="47" t="s">
+      <c r="AD4" s="43"/>
+      <c r="AE4" s="42" t="s">
         <v>5</v>
       </c>
       <c r="AF4" s="41"/>
@@ -1218,8 +1238,8 @@
       <c r="AH4" s="41"/>
       <c r="AI4" s="41"/>
       <c r="AJ4" s="41"/>
-      <c r="AK4" s="42"/>
-      <c r="AL4" s="47" t="s">
+      <c r="AK4" s="43"/>
+      <c r="AL4" s="42" t="s">
         <v>6</v>
       </c>
       <c r="AM4" s="41"/>
@@ -1227,8 +1247,8 @@
       <c r="AO4" s="41"/>
       <c r="AP4" s="41"/>
       <c r="AQ4" s="41"/>
-      <c r="AR4" s="42"/>
-      <c r="AS4" s="47" t="s">
+      <c r="AR4" s="43"/>
+      <c r="AS4" s="42" t="s">
         <v>6</v>
       </c>
       <c r="AT4" s="41"/>
@@ -1236,8 +1256,8 @@
       <c r="AV4" s="41"/>
       <c r="AW4" s="41"/>
       <c r="AX4" s="41"/>
-      <c r="AY4" s="42"/>
-      <c r="AZ4" s="47" t="s">
+      <c r="AY4" s="43"/>
+      <c r="AZ4" s="42" t="s">
         <v>7</v>
       </c>
       <c r="BA4" s="41"/>
@@ -1245,8 +1265,8 @@
       <c r="BC4" s="41"/>
       <c r="BD4" s="41"/>
       <c r="BE4" s="41"/>
-      <c r="BF4" s="42"/>
-      <c r="BG4" s="47" t="s">
+      <c r="BF4" s="43"/>
+      <c r="BG4" s="42" t="s">
         <v>8</v>
       </c>
       <c r="BH4" s="41"/>
@@ -1254,23 +1274,23 @@
       <c r="BJ4" s="41"/>
       <c r="BK4" s="41"/>
       <c r="BL4" s="41"/>
-      <c r="BM4" s="42"/>
+      <c r="BM4" s="43"/>
     </row>
     <row r="5" spans="1:65" ht="15" x14ac:dyDescent="0.25">
       <c r="A5" s="24"/>
-      <c r="B5" s="44" t="s">
+      <c r="B5" s="45" t="s">
         <v>9</v>
       </c>
       <c r="C5" s="41"/>
-      <c r="D5" s="45" t="s">
+      <c r="D5" s="46" t="s">
         <v>18</v>
       </c>
-      <c r="E5" s="46"/>
+      <c r="E5" s="39"/>
       <c r="F5" s="24"/>
       <c r="G5" s="24"/>
       <c r="H5" s="24"/>
       <c r="I5" s="24"/>
-      <c r="J5" s="40">
+      <c r="J5" s="44">
         <f>J6</f>
         <v>44641</v>
       </c>
@@ -1279,8 +1299,8 @@
       <c r="M5" s="41"/>
       <c r="N5" s="41"/>
       <c r="O5" s="41"/>
-      <c r="P5" s="42"/>
-      <c r="Q5" s="40">
+      <c r="P5" s="43"/>
+      <c r="Q5" s="44">
         <f>Q6</f>
         <v>44648</v>
       </c>
@@ -1289,8 +1309,8 @@
       <c r="T5" s="41"/>
       <c r="U5" s="41"/>
       <c r="V5" s="41"/>
-      <c r="W5" s="42"/>
-      <c r="X5" s="40">
+      <c r="W5" s="43"/>
+      <c r="X5" s="44">
         <f>X6</f>
         <v>44655</v>
       </c>
@@ -1299,8 +1319,8 @@
       <c r="AA5" s="41"/>
       <c r="AB5" s="41"/>
       <c r="AC5" s="41"/>
-      <c r="AD5" s="42"/>
-      <c r="AE5" s="40">
+      <c r="AD5" s="43"/>
+      <c r="AE5" s="44">
         <f>AE6</f>
         <v>44662</v>
       </c>
@@ -1309,8 +1329,8 @@
       <c r="AH5" s="41"/>
       <c r="AI5" s="41"/>
       <c r="AJ5" s="41"/>
-      <c r="AK5" s="42"/>
-      <c r="AL5" s="40">
+      <c r="AK5" s="43"/>
+      <c r="AL5" s="44">
         <f>AL6</f>
         <v>44669</v>
       </c>
@@ -1319,8 +1339,8 @@
       <c r="AO5" s="41"/>
       <c r="AP5" s="41"/>
       <c r="AQ5" s="41"/>
-      <c r="AR5" s="42"/>
-      <c r="AS5" s="40">
+      <c r="AR5" s="43"/>
+      <c r="AS5" s="44">
         <f>AS6</f>
         <v>44676</v>
       </c>
@@ -1329,8 +1349,8 @@
       <c r="AV5" s="41"/>
       <c r="AW5" s="41"/>
       <c r="AX5" s="41"/>
-      <c r="AY5" s="42"/>
-      <c r="AZ5" s="40">
+      <c r="AY5" s="43"/>
+      <c r="AZ5" s="44">
         <f>AZ6</f>
         <v>44683</v>
       </c>
@@ -1339,8 +1359,8 @@
       <c r="BC5" s="41"/>
       <c r="BD5" s="41"/>
       <c r="BE5" s="41"/>
-      <c r="BF5" s="42"/>
-      <c r="BG5" s="40">
+      <c r="BF5" s="43"/>
+      <c r="BG5" s="44">
         <f>BG6</f>
         <v>44690</v>
       </c>
@@ -1349,7 +1369,7 @@
       <c r="BJ5" s="41"/>
       <c r="BK5" s="41"/>
       <c r="BL5" s="41"/>
-      <c r="BM5" s="42"/>
+      <c r="BM5" s="43"/>
     </row>
     <row r="6" spans="1:65" ht="15" x14ac:dyDescent="0.25">
       <c r="A6" s="24"/>
@@ -2276,16 +2296,16 @@
         <v>2.1</v>
       </c>
       <c r="B15" s="13" t="s">
-        <v>17</v>
-      </c>
-      <c r="C15" s="13"/>
-      <c r="D15" s="14">
-        <f>$D$14</f>
-        <v>44655</v>
-      </c>
-      <c r="E15" s="15">
-        <f t="shared" ref="E15:E19" si="7">D15+F15-1</f>
-        <v>44659</v>
+        <v>54</v>
+      </c>
+      <c r="C15" s="13" t="s">
+        <v>49</v>
+      </c>
+      <c r="D15" s="14" t="s">
+        <v>59</v>
+      </c>
+      <c r="E15" s="15" t="s">
+        <v>60</v>
       </c>
       <c r="F15" s="16">
         <v>5</v>
@@ -2293,9 +2313,9 @@
       <c r="G15" s="17">
         <v>0</v>
       </c>
-      <c r="H15" s="18">
+      <c r="H15" s="18" t="e">
         <f t="shared" si="5"/>
-        <v>5</v>
+        <v>#VALUE!</v>
       </c>
       <c r="I15" s="18"/>
       <c r="J15" s="32"/>
@@ -2361,16 +2381,16 @@
         <v>2.2</v>
       </c>
       <c r="B16" s="13" t="s">
-        <v>17</v>
-      </c>
-      <c r="C16" s="13"/>
-      <c r="D16" s="14">
-        <f t="shared" ref="D16:D19" si="8">WORKDAY(E15,1)</f>
-        <v>44662</v>
-      </c>
-      <c r="E16" s="15">
-        <f t="shared" si="7"/>
-        <v>44668</v>
+        <v>55</v>
+      </c>
+      <c r="C16" s="13" t="s">
+        <v>27</v>
+      </c>
+      <c r="D16" s="14" t="s">
+        <v>59</v>
+      </c>
+      <c r="E16" s="15" t="s">
+        <v>60</v>
       </c>
       <c r="F16" s="16">
         <v>7</v>
@@ -2378,9 +2398,9 @@
       <c r="G16" s="17">
         <v>0</v>
       </c>
-      <c r="H16" s="18">
+      <c r="H16" s="18" t="e">
         <f t="shared" si="5"/>
-        <v>5</v>
+        <v>#VALUE!</v>
       </c>
       <c r="I16" s="18"/>
       <c r="J16" s="32"/>
@@ -2446,16 +2466,16 @@
         <v>2.3</v>
       </c>
       <c r="B17" s="13" t="s">
-        <v>17</v>
-      </c>
-      <c r="C17" s="13"/>
-      <c r="D17" s="14">
-        <f t="shared" si="8"/>
-        <v>44669</v>
-      </c>
-      <c r="E17" s="15">
-        <f t="shared" si="7"/>
-        <v>44674</v>
+        <v>56</v>
+      </c>
+      <c r="C17" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="D17" s="14" t="s">
+        <v>59</v>
+      </c>
+      <c r="E17" s="15" t="s">
+        <v>60</v>
       </c>
       <c r="F17" s="16">
         <v>6</v>
@@ -2463,9 +2483,9 @@
       <c r="G17" s="17">
         <v>0</v>
       </c>
-      <c r="H17" s="18">
+      <c r="H17" s="18" t="e">
         <f t="shared" si="5"/>
-        <v>5</v>
+        <v>#VALUE!</v>
       </c>
       <c r="I17" s="18"/>
       <c r="J17" s="32"/>
@@ -2534,13 +2554,11 @@
         <v>17</v>
       </c>
       <c r="C18" s="13"/>
-      <c r="D18" s="14">
-        <f t="shared" si="8"/>
-        <v>44676</v>
-      </c>
-      <c r="E18" s="15">
-        <f t="shared" si="7"/>
-        <v>44677</v>
+      <c r="D18" s="14" t="s">
+        <v>59</v>
+      </c>
+      <c r="E18" s="15" t="s">
+        <v>60</v>
       </c>
       <c r="F18" s="16">
         <v>2</v>
@@ -2548,9 +2566,9 @@
       <c r="G18" s="17">
         <v>0</v>
       </c>
-      <c r="H18" s="18">
+      <c r="H18" s="18" t="e">
         <f t="shared" si="5"/>
-        <v>2</v>
+        <v>#VALUE!</v>
       </c>
       <c r="I18" s="18"/>
       <c r="J18" s="32"/>
@@ -2616,16 +2634,16 @@
         <v>2.5</v>
       </c>
       <c r="B19" s="13" t="s">
-        <v>17</v>
-      </c>
-      <c r="C19" s="13"/>
-      <c r="D19" s="14">
-        <f t="shared" si="8"/>
-        <v>44678</v>
-      </c>
-      <c r="E19" s="15">
-        <f t="shared" si="7"/>
-        <v>44681</v>
+        <v>57</v>
+      </c>
+      <c r="C19" s="13" t="s">
+        <v>58</v>
+      </c>
+      <c r="D19" s="14" t="s">
+        <v>59</v>
+      </c>
+      <c r="E19" s="15" t="s">
+        <v>60</v>
       </c>
       <c r="F19" s="16">
         <v>4</v>
@@ -2633,9 +2651,9 @@
       <c r="G19" s="17">
         <v>0</v>
       </c>
-      <c r="H19" s="18">
+      <c r="H19" s="18" t="e">
         <f t="shared" si="5"/>
-        <v>3</v>
+        <v>#VALUE!</v>
       </c>
       <c r="I19" s="18"/>
       <c r="J19" s="32"/>
@@ -2718,7 +2736,7 @@
         <v>1</v>
       </c>
       <c r="H20" s="10">
-        <f t="shared" ref="H20:H25" si="9">NETWORKDAYS(D20,E20)</f>
+        <f t="shared" ref="H20:H25" si="7">NETWORKDAYS(D20,E20)</f>
         <v>11</v>
       </c>
       <c r="I20" s="10"/>
@@ -2781,7 +2799,7 @@
     </row>
     <row r="21" spans="1:65" ht="15" x14ac:dyDescent="0.25">
       <c r="A21" s="12" t="str">
-        <f t="shared" ref="A21:A25" ca="1" si="10">IF(ISERROR(VALUE(SUBSTITUTE(OFFSET(A21,-1,0,1,1),".",""))),"0.1",IF(ISERROR(FIND("`",SUBSTITUTE(OFFSET(A21,-1,0,1,1),".","`",1))),OFFSET(A21,-1,0,1,1)&amp;".1",LEFT(OFFSET(A21,-1,0,1,1),FIND("`",SUBSTITUTE(OFFSET(A21,-1,0,1,1),".","`",1)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(OFFSET(A21,-1,0,1,1),".","`",2))),VALUE(RIGHT(OFFSET(A21,-1,0,1,1),LEN(OFFSET(A21,-1,0,1,1))-FIND("`",SUBSTITUTE(OFFSET(A21,-1,0,1,1),".","`",1))))+1,VALUE(MID(OFFSET(A21,-1,0,1,1),FIND("`",SUBSTITUTE(OFFSET(A21,-1,0,1,1),".","`",1))+1,(FIND("`",SUBSTITUTE(OFFSET(A21,-1,0,1,1),".","`",2))-FIND("`",SUBSTITUTE(OFFSET(A21,-1,0,1,1),".","`",1))-1)))+1)))</f>
+        <f t="shared" ref="A21:A25" ca="1" si="8">IF(ISERROR(VALUE(SUBSTITUTE(OFFSET(A21,-1,0,1,1),".",""))),"0.1",IF(ISERROR(FIND("`",SUBSTITUTE(OFFSET(A21,-1,0,1,1),".","`",1))),OFFSET(A21,-1,0,1,1)&amp;".1",LEFT(OFFSET(A21,-1,0,1,1),FIND("`",SUBSTITUTE(OFFSET(A21,-1,0,1,1),".","`",1)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(OFFSET(A21,-1,0,1,1),".","`",2))),VALUE(RIGHT(OFFSET(A21,-1,0,1,1),LEN(OFFSET(A21,-1,0,1,1))-FIND("`",SUBSTITUTE(OFFSET(A21,-1,0,1,1),".","`",1))))+1,VALUE(MID(OFFSET(A21,-1,0,1,1),FIND("`",SUBSTITUTE(OFFSET(A21,-1,0,1,1),".","`",1))+1,(FIND("`",SUBSTITUTE(OFFSET(A21,-1,0,1,1),".","`",2))-FIND("`",SUBSTITUTE(OFFSET(A21,-1,0,1,1),".","`",1))-1)))+1)))</f>
         <v>3.1</v>
       </c>
       <c r="B21" s="13" t="s">
@@ -2795,7 +2813,7 @@
         <v>44648</v>
       </c>
       <c r="E21" s="15">
-        <f t="shared" ref="E21:E25" si="11">D21+F21-1</f>
+        <f t="shared" ref="E21:E25" si="9">D21+F21-1</f>
         <v>44649</v>
       </c>
       <c r="F21" s="16">
@@ -2805,7 +2823,7 @@
         <v>1</v>
       </c>
       <c r="H21" s="18">
-        <f t="shared" si="9"/>
+        <f t="shared" si="7"/>
         <v>2</v>
       </c>
       <c r="I21" s="18"/>
@@ -2868,7 +2886,7 @@
     </row>
     <row r="22" spans="1:65" ht="30" x14ac:dyDescent="0.25">
       <c r="A22" s="12" t="str">
-        <f t="shared" ca="1" si="10"/>
+        <f t="shared" ca="1" si="8"/>
         <v>3.2</v>
       </c>
       <c r="B22" s="19" t="s">
@@ -2878,11 +2896,11 @@
         <v>30</v>
       </c>
       <c r="D22" s="14">
-        <f t="shared" ref="D22:D25" si="12">WORKDAY.INTL(E21,1,"0000001")</f>
+        <f t="shared" ref="D22:D25" si="10">WORKDAY.INTL(E21,1,"0000001")</f>
         <v>44650</v>
       </c>
       <c r="E22" s="15">
-        <f t="shared" si="11"/>
+        <f t="shared" si="9"/>
         <v>44651</v>
       </c>
       <c r="F22" s="16">
@@ -2892,7 +2910,7 @@
         <v>1</v>
       </c>
       <c r="H22" s="18">
-        <f t="shared" si="9"/>
+        <f t="shared" si="7"/>
         <v>2</v>
       </c>
       <c r="I22" s="18"/>
@@ -2955,21 +2973,21 @@
     </row>
     <row r="23" spans="1:65" ht="15" x14ac:dyDescent="0.25">
       <c r="A23" s="12" t="str">
-        <f t="shared" ca="1" si="10"/>
+        <f t="shared" ca="1" si="8"/>
         <v>3.3</v>
       </c>
       <c r="B23" s="13" t="s">
         <v>37</v>
       </c>
-      <c r="C23" s="37" t="s">
+      <c r="C23" s="47" t="s">
         <v>18</v>
       </c>
       <c r="D23" s="14">
-        <f t="shared" si="12"/>
+        <f t="shared" si="10"/>
         <v>44652</v>
       </c>
       <c r="E23" s="15">
-        <f t="shared" si="11"/>
+        <f t="shared" si="9"/>
         <v>44656</v>
       </c>
       <c r="F23" s="16">
@@ -2979,7 +2997,7 @@
         <v>1</v>
       </c>
       <c r="H23" s="18">
-        <f t="shared" si="9"/>
+        <f t="shared" si="7"/>
         <v>3</v>
       </c>
       <c r="I23" s="18"/>
@@ -3042,19 +3060,19 @@
     </row>
     <row r="24" spans="1:65" ht="30" x14ac:dyDescent="0.25">
       <c r="A24" s="12" t="str">
-        <f t="shared" ca="1" si="10"/>
+        <f t="shared" ca="1" si="8"/>
         <v>3.4</v>
       </c>
       <c r="B24" s="19" t="s">
         <v>38</v>
       </c>
-      <c r="C24" s="38"/>
+      <c r="C24" s="48"/>
       <c r="D24" s="14">
-        <f t="shared" si="12"/>
+        <f t="shared" si="10"/>
         <v>44657</v>
       </c>
       <c r="E24" s="15">
-        <f t="shared" si="11"/>
+        <f t="shared" si="9"/>
         <v>44661</v>
       </c>
       <c r="F24" s="16">
@@ -3064,7 +3082,7 @@
         <v>1</v>
       </c>
       <c r="H24" s="18">
-        <f t="shared" si="9"/>
+        <f t="shared" si="7"/>
         <v>3</v>
       </c>
       <c r="I24" s="18"/>
@@ -3127,19 +3145,19 @@
     </row>
     <row r="25" spans="1:65" ht="30" x14ac:dyDescent="0.25">
       <c r="A25" s="12" t="str">
-        <f t="shared" ca="1" si="10"/>
+        <f t="shared" ca="1" si="8"/>
         <v>3.5</v>
       </c>
       <c r="B25" s="19" t="s">
         <v>39</v>
       </c>
-      <c r="C25" s="39"/>
+      <c r="C25" s="49"/>
       <c r="D25" s="14">
-        <f t="shared" si="12"/>
+        <f t="shared" si="10"/>
         <v>44662</v>
       </c>
       <c r="E25" s="15">
-        <f t="shared" si="11"/>
+        <f t="shared" si="9"/>
         <v>44662</v>
       </c>
       <c r="F25" s="16">
@@ -3149,7 +3167,7 @@
         <v>1</v>
       </c>
       <c r="H25" s="18">
-        <f t="shared" si="9"/>
+        <f t="shared" si="7"/>
         <v>1</v>
       </c>
       <c r="I25" s="18"/>
@@ -3232,7 +3250,7 @@
       </c>
       <c r="G26" s="11"/>
       <c r="H26" s="10">
-        <f t="shared" ref="H26:H35" si="13">NETWORKDAYS(D26,E26)</f>
+        <f t="shared" ref="H26:H35" si="11">NETWORKDAYS(D26,E26)</f>
         <v>31</v>
       </c>
       <c r="I26" s="10"/>
@@ -3295,13 +3313,13 @@
     </row>
     <row r="27" spans="1:65" ht="30" x14ac:dyDescent="0.25">
       <c r="A27" s="12" t="str">
-        <f t="shared" ref="A27:A35" ca="1" si="14">IF(ISERROR(VALUE(SUBSTITUTE(OFFSET(A27,-1,0,1,1),".",""))),"0.1",IF(ISERROR(FIND("`",SUBSTITUTE(OFFSET(A27,-1,0,1,1),".","`",1))),OFFSET(A27,-1,0,1,1)&amp;".1",LEFT(OFFSET(A27,-1,0,1,1),FIND("`",SUBSTITUTE(OFFSET(A27,-1,0,1,1),".","`",1)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(OFFSET(A27,-1,0,1,1),".","`",2))),VALUE(RIGHT(OFFSET(A27,-1,0,1,1),LEN(OFFSET(A27,-1,0,1,1))-FIND("`",SUBSTITUTE(OFFSET(A27,-1,0,1,1),".","`",1))))+1,VALUE(MID(OFFSET(A27,-1,0,1,1),FIND("`",SUBSTITUTE(OFFSET(A27,-1,0,1,1),".","`",1))+1,(FIND("`",SUBSTITUTE(OFFSET(A27,-1,0,1,1),".","`",2))-FIND("`",SUBSTITUTE(OFFSET(A27,-1,0,1,1),".","`",1))-1)))+1)))</f>
+        <f t="shared" ref="A27:A35" ca="1" si="12">IF(ISERROR(VALUE(SUBSTITUTE(OFFSET(A27,-1,0,1,1),".",""))),"0.1",IF(ISERROR(FIND("`",SUBSTITUTE(OFFSET(A27,-1,0,1,1),".","`",1))),OFFSET(A27,-1,0,1,1)&amp;".1",LEFT(OFFSET(A27,-1,0,1,1),FIND("`",SUBSTITUTE(OFFSET(A27,-1,0,1,1),".","`",1)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(OFFSET(A27,-1,0,1,1),".","`",2))),VALUE(RIGHT(OFFSET(A27,-1,0,1,1),LEN(OFFSET(A27,-1,0,1,1))-FIND("`",SUBSTITUTE(OFFSET(A27,-1,0,1,1),".","`",1))))+1,VALUE(MID(OFFSET(A27,-1,0,1,1),FIND("`",SUBSTITUTE(OFFSET(A27,-1,0,1,1),".","`",1))+1,(FIND("`",SUBSTITUTE(OFFSET(A27,-1,0,1,1),".","`",2))-FIND("`",SUBSTITUTE(OFFSET(A27,-1,0,1,1),".","`",1))-1)))+1)))</f>
         <v>4.1</v>
       </c>
       <c r="B27" s="19" t="s">
         <v>40</v>
       </c>
-      <c r="C27" s="37" t="s">
+      <c r="C27" s="47" t="s">
         <v>18</v>
       </c>
       <c r="D27" s="14">
@@ -3309,7 +3327,7 @@
         <v>44641</v>
       </c>
       <c r="E27" s="15">
-        <f t="shared" ref="E27:E35" si="15">D27+F27-1</f>
+        <f t="shared" ref="E27:E35" si="13">D27+F27-1</f>
         <v>44642</v>
       </c>
       <c r="F27" s="16">
@@ -3319,7 +3337,7 @@
         <v>1</v>
       </c>
       <c r="H27" s="18">
-        <f t="shared" si="13"/>
+        <f t="shared" si="11"/>
         <v>2</v>
       </c>
       <c r="I27" s="18"/>
@@ -3382,19 +3400,19 @@
     </row>
     <row r="28" spans="1:65" ht="15" x14ac:dyDescent="0.25">
       <c r="A28" s="12" t="str">
-        <f t="shared" ca="1" si="14"/>
+        <f t="shared" ca="1" si="12"/>
         <v>4.2</v>
       </c>
       <c r="B28" s="13" t="s">
         <v>41</v>
       </c>
-      <c r="C28" s="38"/>
+      <c r="C28" s="48"/>
       <c r="D28" s="14">
-        <f t="shared" ref="D28:D35" si="16">E27+1</f>
+        <f t="shared" ref="D28:D35" si="14">E27+1</f>
         <v>44643</v>
       </c>
       <c r="E28" s="15">
-        <f t="shared" si="15"/>
+        <f t="shared" si="13"/>
         <v>44647</v>
       </c>
       <c r="F28" s="16">
@@ -3404,7 +3422,7 @@
         <v>1</v>
       </c>
       <c r="H28" s="18">
-        <f t="shared" si="13"/>
+        <f t="shared" si="11"/>
         <v>3</v>
       </c>
       <c r="I28" s="18"/>
@@ -3467,19 +3485,19 @@
     </row>
     <row r="29" spans="1:65" ht="15" x14ac:dyDescent="0.25">
       <c r="A29" s="12" t="str">
-        <f t="shared" ca="1" si="14"/>
+        <f t="shared" ca="1" si="12"/>
         <v>4.3</v>
       </c>
       <c r="B29" s="13" t="s">
         <v>42</v>
       </c>
-      <c r="C29" s="39"/>
+      <c r="C29" s="49"/>
       <c r="D29" s="14">
-        <f t="shared" si="16"/>
+        <f t="shared" si="14"/>
         <v>44648</v>
       </c>
       <c r="E29" s="15">
-        <f t="shared" si="15"/>
+        <f t="shared" si="13"/>
         <v>44657</v>
       </c>
       <c r="F29" s="16">
@@ -3489,7 +3507,7 @@
         <v>0.5</v>
       </c>
       <c r="H29" s="18">
-        <f t="shared" si="13"/>
+        <f t="shared" si="11"/>
         <v>8</v>
       </c>
       <c r="I29" s="18"/>
@@ -3552,21 +3570,21 @@
     </row>
     <row r="30" spans="1:65" ht="15" x14ac:dyDescent="0.25">
       <c r="A30" s="12" t="str">
-        <f t="shared" ca="1" si="14"/>
+        <f t="shared" ca="1" si="12"/>
         <v>4.4</v>
       </c>
       <c r="B30" s="13" t="s">
         <v>43</v>
       </c>
-      <c r="C30" s="37" t="s">
+      <c r="C30" s="47" t="s">
         <v>31</v>
       </c>
       <c r="D30" s="14">
-        <f t="shared" si="16"/>
+        <f t="shared" si="14"/>
         <v>44658</v>
       </c>
       <c r="E30" s="15">
-        <f t="shared" si="15"/>
+        <f t="shared" si="13"/>
         <v>44662</v>
       </c>
       <c r="F30" s="16">
@@ -3576,7 +3594,7 @@
         <v>0.7</v>
       </c>
       <c r="H30" s="18">
-        <f t="shared" si="13"/>
+        <f t="shared" si="11"/>
         <v>3</v>
       </c>
       <c r="I30" s="18"/>
@@ -3639,19 +3657,19 @@
     </row>
     <row r="31" spans="1:65" ht="15" x14ac:dyDescent="0.25">
       <c r="A31" s="12" t="str">
-        <f t="shared" ca="1" si="14"/>
+        <f t="shared" ca="1" si="12"/>
         <v>4.5</v>
       </c>
       <c r="B31" s="13" t="s">
         <v>44</v>
       </c>
-      <c r="C31" s="39"/>
+      <c r="C31" s="49"/>
       <c r="D31" s="14">
-        <f t="shared" si="16"/>
+        <f t="shared" si="14"/>
         <v>44663</v>
       </c>
       <c r="E31" s="15">
-        <f t="shared" si="15"/>
+        <f t="shared" si="13"/>
         <v>44667</v>
       </c>
       <c r="F31" s="16">
@@ -3661,7 +3679,7 @@
         <v>0</v>
       </c>
       <c r="H31" s="18">
-        <f t="shared" si="13"/>
+        <f t="shared" si="11"/>
         <v>4</v>
       </c>
       <c r="I31" s="18"/>
@@ -3724,7 +3742,7 @@
     </row>
     <row r="32" spans="1:65" ht="15" x14ac:dyDescent="0.25">
       <c r="A32" s="12" t="str">
-        <f t="shared" ca="1" si="14"/>
+        <f t="shared" ca="1" si="12"/>
         <v>4.6</v>
       </c>
       <c r="B32" s="13" t="s">
@@ -3734,11 +3752,11 @@
         <v>30</v>
       </c>
       <c r="D32" s="14">
-        <f t="shared" si="16"/>
+        <f t="shared" si="14"/>
         <v>44668</v>
       </c>
       <c r="E32" s="15">
-        <f t="shared" si="15"/>
+        <f t="shared" si="13"/>
         <v>44672</v>
       </c>
       <c r="F32" s="16">
@@ -3748,7 +3766,7 @@
         <v>0</v>
       </c>
       <c r="H32" s="18">
-        <f t="shared" si="13"/>
+        <f t="shared" si="11"/>
         <v>4</v>
       </c>
       <c r="I32" s="18"/>
@@ -3811,7 +3829,7 @@
     </row>
     <row r="33" spans="1:65" ht="15" x14ac:dyDescent="0.25">
       <c r="A33" s="12" t="str">
-        <f t="shared" ca="1" si="14"/>
+        <f t="shared" ca="1" si="12"/>
         <v>4.7</v>
       </c>
       <c r="B33" s="13" t="s">
@@ -3821,11 +3839,11 @@
         <v>25</v>
       </c>
       <c r="D33" s="14">
-        <f t="shared" si="16"/>
+        <f t="shared" si="14"/>
         <v>44673</v>
       </c>
       <c r="E33" s="15">
-        <f t="shared" si="15"/>
+        <f t="shared" si="13"/>
         <v>44677</v>
       </c>
       <c r="F33" s="16">
@@ -3835,7 +3853,7 @@
         <v>0</v>
       </c>
       <c r="H33" s="18">
-        <f t="shared" si="13"/>
+        <f t="shared" si="11"/>
         <v>3</v>
       </c>
       <c r="I33" s="18"/>
@@ -3905,11 +3923,11 @@
         <v>49</v>
       </c>
       <c r="D34" s="14">
-        <f t="shared" si="16"/>
+        <f t="shared" si="14"/>
         <v>44678</v>
       </c>
       <c r="E34" s="15">
-        <f t="shared" si="15"/>
+        <f t="shared" si="13"/>
         <v>44682</v>
       </c>
       <c r="F34" s="16">
@@ -3919,7 +3937,7 @@
         <v>0</v>
       </c>
       <c r="H34" s="18">
-        <f t="shared" si="13"/>
+        <f t="shared" si="11"/>
         <v>3</v>
       </c>
       <c r="I34" s="18"/>
@@ -3982,7 +4000,7 @@
     </row>
     <row r="35" spans="1:65" ht="15" x14ac:dyDescent="0.25">
       <c r="A35" s="12" t="str">
-        <f t="shared" ca="1" si="14"/>
+        <f t="shared" ca="1" si="12"/>
         <v>0.1</v>
       </c>
       <c r="B35" s="13" t="s">
@@ -3992,11 +4010,11 @@
         <v>27</v>
       </c>
       <c r="D35" s="14">
-        <f t="shared" si="16"/>
+        <f t="shared" si="14"/>
         <v>44683</v>
       </c>
       <c r="E35" s="15">
-        <f t="shared" si="15"/>
+        <f t="shared" si="13"/>
         <v>44683</v>
       </c>
       <c r="F35" s="16">
@@ -4006,7 +4024,7 @@
         <v>0</v>
       </c>
       <c r="H35" s="18">
-        <f t="shared" si="13"/>
+        <f t="shared" si="11"/>
         <v>1</v>
       </c>
       <c r="I35" s="18"/>
@@ -4088,7 +4106,7 @@
       </c>
       <c r="G36" s="11"/>
       <c r="H36" s="10">
-        <f t="shared" ref="H36:H41" si="17">NETWORKDAYS(D36,E36)</f>
+        <f t="shared" ref="H36:H41" si="15">NETWORKDAYS(D36,E36)</f>
         <v>10</v>
       </c>
       <c r="I36" s="10"/>
@@ -4151,7 +4169,7 @@
     </row>
     <row r="37" spans="1:65" ht="15" x14ac:dyDescent="0.25">
       <c r="A37" s="12" t="str">
-        <f t="shared" ref="A37:A41" ca="1" si="18">IF(ISERROR(VALUE(SUBSTITUTE(OFFSET(A37,-1,0,1,1),".",""))),"0.1",IF(ISERROR(FIND("`",SUBSTITUTE(OFFSET(A37,-1,0,1,1),".","`",1))),OFFSET(A37,-1,0,1,1)&amp;".1",LEFT(OFFSET(A37,-1,0,1,1),FIND("`",SUBSTITUTE(OFFSET(A37,-1,0,1,1),".","`",1)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(OFFSET(A37,-1,0,1,1),".","`",2))),VALUE(RIGHT(OFFSET(A37,-1,0,1,1),LEN(OFFSET(A37,-1,0,1,1))-FIND("`",SUBSTITUTE(OFFSET(A37,-1,0,1,1),".","`",1))))+1,VALUE(MID(OFFSET(A37,-1,0,1,1),FIND("`",SUBSTITUTE(OFFSET(A37,-1,0,1,1),".","`",1))+1,(FIND("`",SUBSTITUTE(OFFSET(A37,-1,0,1,1),".","`",2))-FIND("`",SUBSTITUTE(OFFSET(A37,-1,0,1,1),".","`",1))-1)))+1)))</f>
+        <f t="shared" ref="A37:A41" ca="1" si="16">IF(ISERROR(VALUE(SUBSTITUTE(OFFSET(A37,-1,0,1,1),".",""))),"0.1",IF(ISERROR(FIND("`",SUBSTITUTE(OFFSET(A37,-1,0,1,1),".","`",1))),OFFSET(A37,-1,0,1,1)&amp;".1",LEFT(OFFSET(A37,-1,0,1,1),FIND("`",SUBSTITUTE(OFFSET(A37,-1,0,1,1),".","`",1)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(OFFSET(A37,-1,0,1,1),".","`",2))),VALUE(RIGHT(OFFSET(A37,-1,0,1,1),LEN(OFFSET(A37,-1,0,1,1))-FIND("`",SUBSTITUTE(OFFSET(A37,-1,0,1,1),".","`",1))))+1,VALUE(MID(OFFSET(A37,-1,0,1,1),FIND("`",SUBSTITUTE(OFFSET(A37,-1,0,1,1),".","`",1))+1,(FIND("`",SUBSTITUTE(OFFSET(A37,-1,0,1,1),".","`",2))-FIND("`",SUBSTITUTE(OFFSET(A37,-1,0,1,1),".","`",1))-1)))+1)))</f>
         <v>1.1</v>
       </c>
       <c r="B37" s="13" t="s">
@@ -4165,7 +4183,7 @@
         <v>44683</v>
       </c>
       <c r="E37" s="15">
-        <f t="shared" ref="E37:E41" si="19">D37+F37-1</f>
+        <f t="shared" ref="E37:E41" si="17">D37+F37-1</f>
         <v>44686</v>
       </c>
       <c r="F37" s="16">
@@ -4175,7 +4193,7 @@
         <v>0</v>
       </c>
       <c r="H37" s="18">
-        <f t="shared" si="17"/>
+        <f t="shared" si="15"/>
         <v>4</v>
       </c>
       <c r="I37" s="18"/>
@@ -4238,7 +4256,7 @@
     </row>
     <row r="38" spans="1:65" ht="15" x14ac:dyDescent="0.25">
       <c r="A38" s="12" t="str">
-        <f t="shared" ca="1" si="18"/>
+        <f t="shared" ca="1" si="16"/>
         <v>1.2</v>
       </c>
       <c r="B38" s="13" t="s">
@@ -4248,11 +4266,11 @@
         <v>49</v>
       </c>
       <c r="D38" s="14">
-        <f t="shared" ref="D38:D41" si="20">E37+1</f>
+        <f t="shared" ref="D38:D41" si="18">E37+1</f>
         <v>44687</v>
       </c>
       <c r="E38" s="15">
-        <f t="shared" si="19"/>
+        <f t="shared" si="17"/>
         <v>44690</v>
       </c>
       <c r="F38" s="16">
@@ -4262,7 +4280,7 @@
         <v>0</v>
       </c>
       <c r="H38" s="18">
-        <f t="shared" si="17"/>
+        <f t="shared" si="15"/>
         <v>2</v>
       </c>
       <c r="I38" s="18"/>
@@ -4325,7 +4343,7 @@
     </row>
     <row r="39" spans="1:65" ht="15" x14ac:dyDescent="0.25">
       <c r="A39" s="12" t="str">
-        <f t="shared" ca="1" si="18"/>
+        <f t="shared" ca="1" si="16"/>
         <v>1.3</v>
       </c>
       <c r="B39" s="13" t="s">
@@ -4335,11 +4353,11 @@
         <v>18</v>
       </c>
       <c r="D39" s="14">
-        <f t="shared" si="20"/>
+        <f t="shared" si="18"/>
         <v>44691</v>
       </c>
       <c r="E39" s="15">
-        <f t="shared" si="19"/>
+        <f t="shared" si="17"/>
         <v>44691</v>
       </c>
       <c r="F39" s="16">
@@ -4349,7 +4367,7 @@
         <v>0</v>
       </c>
       <c r="H39" s="18">
-        <f t="shared" si="17"/>
+        <f t="shared" si="15"/>
         <v>1</v>
       </c>
       <c r="I39" s="18"/>
@@ -4412,7 +4430,7 @@
     </row>
     <row r="40" spans="1:65" ht="15" x14ac:dyDescent="0.25">
       <c r="A40" s="12" t="str">
-        <f t="shared" ca="1" si="18"/>
+        <f t="shared" ca="1" si="16"/>
         <v>1.4</v>
       </c>
       <c r="B40" s="13" t="s">
@@ -4420,11 +4438,11 @@
       </c>
       <c r="C40" s="13"/>
       <c r="D40" s="14">
-        <f t="shared" si="20"/>
+        <f t="shared" si="18"/>
         <v>44692</v>
       </c>
       <c r="E40" s="15">
-        <f t="shared" si="19"/>
+        <f t="shared" si="17"/>
         <v>44692</v>
       </c>
       <c r="F40" s="16">
@@ -4434,7 +4452,7 @@
         <v>0</v>
       </c>
       <c r="H40" s="18">
-        <f t="shared" si="17"/>
+        <f t="shared" si="15"/>
         <v>1</v>
       </c>
       <c r="I40" s="18"/>
@@ -4497,7 +4515,7 @@
     </row>
     <row r="41" spans="1:65" ht="15" x14ac:dyDescent="0.25">
       <c r="A41" s="12" t="str">
-        <f t="shared" ca="1" si="18"/>
+        <f t="shared" ca="1" si="16"/>
         <v>1.5</v>
       </c>
       <c r="B41" s="13" t="s">
@@ -4505,11 +4523,11 @@
       </c>
       <c r="C41" s="13"/>
       <c r="D41" s="14">
-        <f t="shared" si="20"/>
+        <f t="shared" si="18"/>
         <v>44693</v>
       </c>
       <c r="E41" s="15">
-        <f t="shared" si="19"/>
+        <f t="shared" si="17"/>
         <v>44693</v>
       </c>
       <c r="F41" s="16">
@@ -4519,7 +4537,7 @@
         <v>0</v>
       </c>
       <c r="H41" s="18">
-        <f t="shared" si="17"/>
+        <f t="shared" si="15"/>
         <v>1</v>
       </c>
       <c r="I41" s="18"/>
@@ -4716,13 +4734,11 @@
     </row>
   </sheetData>
   <mergeCells count="25">
-    <mergeCell ref="D1:BM1"/>
-    <mergeCell ref="D4:E4"/>
-    <mergeCell ref="F4:G4"/>
-    <mergeCell ref="J4:P4"/>
-    <mergeCell ref="Q4:W4"/>
-    <mergeCell ref="X4:AD4"/>
-    <mergeCell ref="BG4:BM4"/>
+    <mergeCell ref="C23:C25"/>
+    <mergeCell ref="C27:C29"/>
+    <mergeCell ref="C30:C31"/>
+    <mergeCell ref="AL5:AR5"/>
+    <mergeCell ref="AS5:AY5"/>
     <mergeCell ref="AZ5:BF5"/>
     <mergeCell ref="BG5:BM5"/>
     <mergeCell ref="B4:C4"/>
@@ -4736,11 +4752,13 @@
     <mergeCell ref="AL4:AR4"/>
     <mergeCell ref="AS4:AY4"/>
     <mergeCell ref="AZ4:BF4"/>
-    <mergeCell ref="C23:C25"/>
-    <mergeCell ref="C27:C29"/>
-    <mergeCell ref="C30:C31"/>
-    <mergeCell ref="AL5:AR5"/>
-    <mergeCell ref="AS5:AY5"/>
+    <mergeCell ref="D1:BM1"/>
+    <mergeCell ref="D4:E4"/>
+    <mergeCell ref="F4:G4"/>
+    <mergeCell ref="J4:P4"/>
+    <mergeCell ref="Q4:W4"/>
+    <mergeCell ref="X4:AD4"/>
+    <mergeCell ref="BG4:BM4"/>
   </mergeCells>
   <conditionalFormatting sqref="J6:BM7">
     <cfRule type="expression" dxfId="3" priority="1">

</xml_diff>